<commit_message>
Update Daily Work Progress_xen_zaki.xlsx
</commit_message>
<xml_diff>
--- a/Xen Jakaria/Daily Work Progress_xen_zaki.xlsx
+++ b/Xen Jakaria/Daily Work Progress_xen_zaki.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Design-8\Designs_All\Xen Jakaria\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Nane:</t>
   </si>
@@ -120,12 +115,15 @@
   </si>
   <si>
     <t>Regulator Drafting Program:PLAN Drawing:Barrel Part</t>
+  </si>
+  <si>
+    <t>Regulator Drafting Program:PLAN Drawing:WingWall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -274,7 +272,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -309,7 +307,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -486,7 +484,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -494,20 +492,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
+    <col min="2" max="2" width="69.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -523,7 +521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -534,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -545,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -556,7 +554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -567,7 +565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -578,7 +576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -589,7 +587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -600,7 +598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -611,7 +609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -622,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
@@ -633,7 +631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -644,7 +642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -655,7 +653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
@@ -666,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>44986</v>
       </c>
@@ -677,7 +675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>44986</v>
       </c>
@@ -688,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>44986</v>
       </c>
@@ -696,6 +694,17 @@
         <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>45017</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily work schedule updated
daily work schedule updated
</commit_message>
<xml_diff>
--- a/Xen Jakaria/Daily Work Progress_xen_zaki.xlsx
+++ b/Xen Jakaria/Daily Work Progress_xen_zaki.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>Nane:</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>Regulator Structural Design Day-4 Coding</t>
+  </si>
+  <si>
+    <t>Regulator Structural Design Day-5 Coding</t>
+  </si>
+  <si>
+    <t>Regulator Structural Design Day-6 Coding</t>
+  </si>
+  <si>
+    <t>Regulator Structural Design Day-7 Coding</t>
   </si>
 </sst>
 </file>
@@ -190,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -217,6 +226,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -510,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,6 +886,54 @@
         <v>5</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>44945</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>44946</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>44947</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A5">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>